<commit_message>
Updated the xlsx file with latest information
</commit_message>
<xml_diff>
--- a/mtg_data.xlsx
+++ b/mtg_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code\MTG Analysis\venv\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BDDDBF-4639-4F7B-88D2-5A5352B88E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8EC5D1-7401-4028-8B41-456CEF640A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="25">
   <si>
     <t>game_id</t>
   </si>
@@ -488,20 +488,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
-    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +522,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -541,7 +541,7 @@
       <c r="H2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -560,7 +560,7 @@
       <c r="H3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -579,7 +579,7 @@
       <c r="H4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -597,7 +597,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -615,7 +615,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -633,7 +633,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -650,7 +650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -684,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -701,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -718,7 +718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -752,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -769,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -803,7 +803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -820,7 +820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -837,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -871,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>7</v>
       </c>
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>7</v>
       </c>
@@ -905,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -922,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>7</v>
       </c>
@@ -939,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>8</v>
       </c>
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>8</v>
       </c>
@@ -973,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -990,7 +990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>8</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>9</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>9</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>9</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>10</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>10</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>10</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>10</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>11</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>11</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>11</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>11</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>12</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>12</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>12</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>12</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>13</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>13</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>13</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>13</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>14</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>14</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>14</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>14</v>
       </c>
@@ -1413,6 +1413,74 @@
       </c>
       <c r="E53" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>15</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>15</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>15</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>15</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the xlsx file with the latest information
</commit_message>
<xml_diff>
--- a/mtg_data.xlsx
+++ b/mtg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code\MTG Analysis\venv\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8EC5D1-7401-4028-8B41-456CEF640A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7960516-44B5-41BE-B33C-F5C02835AB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="24">
   <si>
     <t>game_id</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Lord of the Rings</t>
-  </si>
-  <si>
-    <t>Becky</t>
   </si>
   <si>
     <t>Rohan</t>
@@ -488,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +530,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
@@ -552,7 +549,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
@@ -571,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -590,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -608,10 +605,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -620,42 +617,41 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -664,7 +660,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -672,16 +668,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -689,16 +685,16 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -706,33 +702,33 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -740,16 +736,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -757,16 +753,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -774,33 +770,33 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -808,16 +804,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -825,16 +821,16 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,27 +838,27 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>16</v>
@@ -876,16 +872,16 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E22" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,16 +889,16 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,33 +906,33 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -944,16 +940,16 @@
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -961,16 +957,16 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -978,7 +974,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>9</v>
@@ -987,24 +983,24 @@
         <v>12</v>
       </c>
       <c r="E28" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,16 +1008,16 @@
         <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,50 +1025,50 @@
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E31" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E32" s="1">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,16 +1076,16 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E34" s="1">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1097,30 +1093,30 @@
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E35" s="1">
-        <v>3.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -1128,19 +1124,19 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E37" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1148,16 +1144,16 @@
         <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E38" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,50 +1161,50 @@
         <v>11</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E39" s="1">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E40" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E41" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,16 +1212,16 @@
         <v>12</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E42" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1233,47 +1229,47 @@
         <v>12</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E43" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E44" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -1284,16 +1280,16 @@
         <v>13</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E46" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1301,47 +1297,47 @@
         <v>13</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E47" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
+        <v>14</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E49" s="1">
         <v>4</v>
@@ -1352,16 +1348,16 @@
         <v>14</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1369,47 +1365,47 @@
         <v>14</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E51" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E52" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E53" s="1">
         <v>3</v>
@@ -1420,16 +1416,16 @@
         <v>15</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E54" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1437,54 +1433,20 @@
         <v>15</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E55" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>15</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>15</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E53" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
+  <autoFilter ref="A1:E55" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
roll back until yesterday, add in draw type and mana colour
</commit_message>
<xml_diff>
--- a/mtg_data.xlsx
+++ b/mtg_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code\MTG Analysis\venv\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7521C24-FE88-4BD4-9EFB-F611093DA03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46B06B5-F85C-4D7F-B1E6-5A650128B89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="39">
   <si>
     <t>game_id</t>
   </si>
@@ -111,6 +111,51 @@
   </si>
   <si>
     <t>Bloomburrow</t>
+  </si>
+  <si>
+    <t>Takir Dragonstorm</t>
+  </si>
+  <si>
+    <t>Jeski Striker</t>
+  </si>
+  <si>
+    <t>Abzan Armour</t>
+  </si>
+  <si>
+    <t>Temur Roar</t>
+  </si>
+  <si>
+    <t>Saultai Anisen</t>
+  </si>
+  <si>
+    <t>Mardu Surge</t>
+  </si>
+  <si>
+    <t>draw_type</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>primary_mana</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -485,20 +530,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="6" max="7" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,12 +559,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -535,10 +582,14 @@
       <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -554,10 +605,14 @@
       <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -573,10 +628,14 @@
       <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -592,9 +651,14 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -610,9 +674,14 @@
       <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -628,8 +697,14 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -645,8 +720,14 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -662,8 +743,14 @@
       <c r="E9" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -679,8 +766,14 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -696,8 +789,14 @@
       <c r="E11" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -713,8 +812,14 @@
       <c r="E12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -730,8 +835,14 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -747,8 +858,14 @@
       <c r="E14" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -764,8 +881,14 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -781,8 +904,14 @@
       <c r="E16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -798,8 +927,14 @@
       <c r="E17" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -815,8 +950,14 @@
       <c r="E18" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -832,8 +973,14 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -849,8 +996,14 @@
       <c r="E20" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -866,8 +1019,14 @@
       <c r="E21" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>7</v>
       </c>
@@ -883,8 +1042,14 @@
       <c r="E22" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>7</v>
       </c>
@@ -900,8 +1065,14 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -917,8 +1088,14 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -934,8 +1111,14 @@
       <c r="E25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>8</v>
       </c>
@@ -951,8 +1134,14 @@
       <c r="E26" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>8</v>
       </c>
@@ -968,8 +1157,14 @@
       <c r="E27" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -985,8 +1180,14 @@
       <c r="E28" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>9</v>
       </c>
@@ -1002,8 +1203,14 @@
       <c r="E29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>9</v>
       </c>
@@ -1019,8 +1226,14 @@
       <c r="E30" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>9</v>
       </c>
@@ -1036,8 +1249,14 @@
       <c r="E31" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>10</v>
       </c>
@@ -1051,10 +1270,16 @@
         <v>19</v>
       </c>
       <c r="E32" s="1">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>10</v>
       </c>
@@ -1068,10 +1293,16 @@
         <v>20</v>
       </c>
       <c r="E33" s="1">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>10</v>
       </c>
@@ -1087,8 +1318,14 @@
       <c r="E34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>10</v>
       </c>
@@ -1104,8 +1341,14 @@
       <c r="E35" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>11</v>
       </c>
@@ -1121,8 +1364,14 @@
       <c r="E36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>11</v>
       </c>
@@ -1138,8 +1387,14 @@
       <c r="E37" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>11</v>
       </c>
@@ -1153,10 +1408,16 @@
         <v>21</v>
       </c>
       <c r="E38" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>11</v>
       </c>
@@ -1170,10 +1431,16 @@
         <v>22</v>
       </c>
       <c r="E39" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>12</v>
       </c>
@@ -1189,8 +1456,14 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>12</v>
       </c>
@@ -1206,8 +1479,14 @@
       <c r="E41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>12</v>
       </c>
@@ -1223,8 +1502,14 @@
       <c r="E42" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>12</v>
       </c>
@@ -1240,8 +1525,14 @@
       <c r="E43" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>13</v>
       </c>
@@ -1257,8 +1548,14 @@
       <c r="E44" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>13</v>
       </c>
@@ -1274,8 +1571,14 @@
       <c r="E45" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>13</v>
       </c>
@@ -1291,8 +1594,14 @@
       <c r="E46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>13</v>
       </c>
@@ -1308,8 +1617,14 @@
       <c r="E47" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>14</v>
       </c>
@@ -1325,8 +1640,14 @@
       <c r="E48" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>14</v>
       </c>
@@ -1342,8 +1663,14 @@
       <c r="E49" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>14</v>
       </c>
@@ -1359,8 +1686,14 @@
       <c r="E50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>14</v>
       </c>
@@ -1376,8 +1709,14 @@
       <c r="E51" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>15</v>
       </c>
@@ -1393,8 +1732,14 @@
       <c r="E52" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>15</v>
       </c>
@@ -1410,8 +1755,14 @@
       <c r="E53" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>15</v>
       </c>
@@ -1427,8 +1778,14 @@
       <c r="E54" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>15</v>
       </c>
@@ -1444,9 +1801,475 @@
       <c r="E55" s="1">
         <v>1</v>
       </c>
+      <c r="F55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>16</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>16</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>16</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>16</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>17</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>17</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="1">
+        <v>3</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>17</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>17</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="1">
+        <v>4</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>18</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="1">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>18</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="1">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>18</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="1">
+        <v>2</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>18</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>19</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="1">
+        <v>3</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>19</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>19</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="1">
+        <v>4</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>19</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E71" s="1">
+        <v>2</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>20</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="1">
+        <v>2</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>20</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="1">
+        <v>3</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>20</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>20</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="1">
+        <v>4</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E55" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
+  <autoFilter ref="A1:G75" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating with latest games
</commit_message>
<xml_diff>
--- a/mtg_data.xlsx
+++ b/mtg_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code\MTG Analysis\venv\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46B06B5-F85C-4D7F-B1E6-5A650128B89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5161BC31-89CF-4089-86F2-AB69AC6C5FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="49">
   <si>
     <t>game_id</t>
   </si>
@@ -156,6 +156,36 @@
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t>Doctor Who</t>
+  </si>
+  <si>
+    <t>Final Fantasy</t>
+  </si>
+  <si>
+    <t>Limit Breaker</t>
+  </si>
+  <si>
+    <t>Blast From the Past</t>
+  </si>
+  <si>
+    <t>Timey Wimey</t>
+  </si>
+  <si>
+    <t>Masters of Evil</t>
+  </si>
+  <si>
+    <t>Paradox Power</t>
+  </si>
+  <si>
+    <t>Counter Blitz</t>
+  </si>
+  <si>
+    <t>Revival Trance</t>
+  </si>
+  <si>
+    <t>Scions &amp; Spell Craft</t>
   </si>
 </sst>
 </file>
@@ -530,16 +560,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="19.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
     <col min="6" max="7" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2268,8 +2296,376 @@
         <v>34</v>
       </c>
     </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>21</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>21</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E77" s="1">
+        <v>3</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>21</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>21</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="1">
+        <v>4</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>22</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>22</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>22</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E82" s="1">
+        <v>3</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>22</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="1">
+        <v>4</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>23</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>23</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E85" s="1">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>23</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>23</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E87" s="1">
+        <v>4</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>24</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>24</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="1">
+        <v>4</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>24</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" s="1">
+        <v>2</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>24</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E91" s="1">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G75" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
+  <autoFilter ref="A1:G91" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated primary colour to technical colour type, i.e. Grixis
</commit_message>
<xml_diff>
--- a/mtg_data.xlsx
+++ b/mtg_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code\MTG Analysis\venv\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5161BC31-89CF-4089-86F2-AB69AC6C5FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0466A73-D9E8-41AD-A010-57990CD20ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="57">
   <si>
     <t>game_id</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Takir Dragonstorm</t>
   </si>
   <si>
-    <t>Jeski Striker</t>
-  </si>
-  <si>
     <t>Abzan Armour</t>
   </si>
   <si>
@@ -143,21 +140,6 @@
     <t>primary_mana</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
     <t>Doctor Who</t>
   </si>
   <si>
@@ -186,6 +168,48 @@
   </si>
   <si>
     <t>Scions &amp; Spell Craft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bant {W} {Blu} {G} </t>
+  </si>
+  <si>
+    <t>Golgari {Black} {G}</t>
+  </si>
+  <si>
+    <t>Gruul {R} {G}</t>
+  </si>
+  <si>
+    <t>Jeskai {W} {Blue} {R}</t>
+  </si>
+  <si>
+    <t>Temur {Blue} {R} {G}</t>
+  </si>
+  <si>
+    <t>Grixis {Blue} {Black} {R}</t>
+  </si>
+  <si>
+    <t>Esper {W} {Blue} {Black}</t>
+  </si>
+  <si>
+    <t>Mardu {W} {Black} {R}</t>
+  </si>
+  <si>
+    <t>Naya {W} {R} {G}</t>
+  </si>
+  <si>
+    <t>Abzan {W} {Black} {G}</t>
+  </si>
+  <si>
+    <t>Simic {Blue} {G}</t>
+  </si>
+  <si>
+    <t>Jeskai Striker</t>
+  </si>
+  <si>
+    <t>Sultai {Blue} {Black} {G}</t>
+  </si>
+  <si>
+    <t>Mono-Black</t>
   </si>
 </sst>
 </file>
@@ -560,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,7 +592,8 @@
   <cols>
     <col min="3" max="3" width="19.08984375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="6" max="7" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -588,10 +613,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -611,10 +636,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -634,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -657,10 +682,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -680,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -703,10 +728,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -726,10 +751,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -749,10 +774,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -772,10 +797,10 @@
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -795,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -818,10 +843,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -841,10 +866,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -864,10 +889,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -887,10 +912,10 @@
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -910,10 +935,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -933,10 +958,10 @@
         <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -956,10 +981,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -979,10 +1004,10 @@
         <v>4</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1002,10 +1027,10 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1025,10 +1050,10 @@
         <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1048,10 +1073,10 @@
         <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1071,10 +1096,10 @@
         <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1094,10 +1119,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1117,10 +1142,10 @@
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1140,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1163,10 +1188,10 @@
         <v>4</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1186,10 +1211,10 @@
         <v>3</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1209,10 +1234,10 @@
         <v>2</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1232,10 +1257,10 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1255,10 +1280,10 @@
         <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1278,10 +1303,10 @@
         <v>3</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1301,10 +1326,10 @@
         <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1324,10 +1349,10 @@
         <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1347,10 +1372,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1370,10 +1395,10 @@
         <v>2</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1393,10 +1418,10 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1416,10 +1441,10 @@
         <v>4</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1439,10 +1464,10 @@
         <v>3</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1462,10 +1487,10 @@
         <v>2</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1485,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1508,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1531,10 +1556,10 @@
         <v>4</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1554,10 +1579,10 @@
         <v>3</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1577,10 +1602,10 @@
         <v>2</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1600,10 +1625,10 @@
         <v>3</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1623,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1646,10 +1671,10 @@
         <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1669,10 +1694,10 @@
         <v>2</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1692,10 +1717,10 @@
         <v>4</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -1715,10 +1740,10 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1738,10 +1763,10 @@
         <v>3</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1761,10 +1786,10 @@
         <v>4</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -1784,10 +1809,10 @@
         <v>3</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -1807,10 +1832,10 @@
         <v>2</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -1830,10 +1855,10 @@
         <v>1</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1853,10 +1878,10 @@
         <v>3</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -1876,10 +1901,10 @@
         <v>2</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -1899,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -1922,10 +1947,10 @@
         <v>4</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -1945,10 +1970,10 @@
         <v>2</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -1968,10 +1993,10 @@
         <v>3</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -1991,10 +2016,10 @@
         <v>1</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2014,10 +2039,10 @@
         <v>4</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2031,16 +2056,16 @@
         <v>24</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2054,16 +2079,16 @@
         <v>24</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E65" s="1">
         <v>3</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2077,16 +2102,16 @@
         <v>24</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E66" s="1">
         <v>2</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2100,16 +2125,16 @@
         <v>24</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E67" s="1">
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2123,16 +2148,16 @@
         <v>24</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E68" s="1">
         <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -2146,16 +2171,16 @@
         <v>24</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E69" s="1">
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -2169,16 +2194,16 @@
         <v>24</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E70" s="1">
         <v>4</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2192,16 +2217,16 @@
         <v>24</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -2215,16 +2240,16 @@
         <v>24</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -2238,16 +2263,16 @@
         <v>24</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E73" s="1">
         <v>3</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2261,16 +2286,16 @@
         <v>24</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E74" s="1">
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -2284,16 +2309,16 @@
         <v>24</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E75" s="1">
         <v>4</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -2304,19 +2329,19 @@
         <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E76" s="1">
         <v>2</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -2327,19 +2352,19 @@
         <v>6</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -2350,19 +2375,19 @@
         <v>7</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E78" s="1">
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -2373,19 +2398,19 @@
         <v>8</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E79" s="1">
         <v>4</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -2396,19 +2421,19 @@
         <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E80" s="1">
         <v>2</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -2419,19 +2444,19 @@
         <v>6</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -2442,19 +2467,19 @@
         <v>7</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -2465,19 +2490,19 @@
         <v>8</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E83" s="1">
         <v>4</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -2488,19 +2513,19 @@
         <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -2511,19 +2536,19 @@
         <v>6</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -2534,19 +2559,19 @@
         <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E86" s="1">
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -2557,19 +2582,19 @@
         <v>8</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E87" s="1">
         <v>4</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -2583,16 +2608,16 @@
         <v>24</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -2606,16 +2631,16 @@
         <v>24</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E89" s="1">
         <v>4</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -2629,16 +2654,16 @@
         <v>24</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E90" s="1">
         <v>2</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -2652,20 +2677,112 @@
         <v>24</v>
       </c>
       <c r="D91" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E91" s="1">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
         <v>25</v>
       </c>
-      <c r="E91" s="1">
-        <v>3</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>34</v>
+      <c r="B92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E92" s="1">
+        <v>4</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>25</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="1">
+        <v>2</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>25</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>25</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="1">
+        <v>3</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G91" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
+  <autoFilter ref="A1:G95" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code to reflect detailed player analysis. Provided colour breakdown. Added recennt games to data. Updated Requirements
</commit_message>
<xml_diff>
--- a/mtg_data.xlsx
+++ b/mtg_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code\MTG Analysis\venv\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0466A73-D9E8-41AD-A010-57990CD20ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B0606-8B29-447B-B1DA-1C842C49207F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1137F1D1-D151-4314-AE7F-A3B4E1F9669F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$103</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="62">
   <si>
     <t>game_id</t>
   </si>
@@ -210,6 +210,21 @@
   </si>
   <si>
     <t>Mono-Black</t>
+  </si>
+  <si>
+    <t>Fallout</t>
+  </si>
+  <si>
+    <t>Mutant Menace</t>
+  </si>
+  <si>
+    <t>Scrappy Survivors</t>
+  </si>
+  <si>
+    <t>Hail, Caeser</t>
+  </si>
+  <si>
+    <t>Science!</t>
   </si>
 </sst>
 </file>
@@ -584,9 +599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}">
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2781,8 +2798,192 @@
         <v>44</v>
       </c>
     </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="1">
+        <v>26</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E96" s="1">
+        <v>4</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>26</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
+        <v>26</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="1">
+        <v>26</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E99" s="1">
+        <v>2</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="1">
+        <v>27</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="1">
+        <v>2</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>27</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" s="1">
+        <v>3</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>27</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>27</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E103" s="1">
+        <v>4</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G95" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
+  <autoFilter ref="A1:G103" xr:uid="{31210DC3-84DF-4463-A036-811DC51179A3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>